<commit_message>
registered time spent on logic based keyword dialog act classifier
</commit_message>
<xml_diff>
--- a/time manegement group 1.xlsx
+++ b/time manegement group 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsm\Documents\AI master\Methods in AI research\group project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gvand\Bureaublad\src\MAIR\MAIR_projectG16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FA8ED5-043F-451C-A36F-1FEFE9011233}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532104BF-602D-4415-8B59-276F0D68DA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Lars</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>first seminar</t>
+  </si>
+  <si>
+    <t>keyword logic-based dialog act classifier</t>
   </si>
 </sst>
 </file>
@@ -360,18 +363,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -388,7 +391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -405,6 +408,14 @@
         <v>2</v>
       </c>
       <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
     </row>

</xml_diff>